<commit_message>
started looking at bureau files
</commit_message>
<xml_diff>
--- a/input/HomeCredit_columns_description.xlsx
+++ b/input/HomeCredit_columns_description.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackr\Documents\kaggle\kaggle-home-credit-default-risk\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8140008_{3A1D68A4-CD85-4E48-B9C7-C3584B429829}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{772C0E52-7264-42E7-93E2-67F9E0642073}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="12810"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HomeCredit_columns_description" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="377">
   <si>
     <t>Table</t>
   </si>
@@ -1159,7 +1159,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1993,12 +1993,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E220"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C64" sqref="C64"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D131" sqref="D131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2024,7 +2024,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>12</v>
       </c>
@@ -2038,7 +2038,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>11</v>
       </c>
@@ -2052,7 +2052,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>13</v>
       </c>
@@ -2066,7 +2066,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>10</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>120</v>
       </c>
@@ -2094,7 +2094,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>119</v>
       </c>
@@ -2108,7 +2108,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>122</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>123</v>
       </c>
@@ -2136,7 +2136,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>121</v>
       </c>
@@ -2150,7 +2150,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>124</v>
       </c>
@@ -2164,7 +2164,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>47</v>
       </c>
@@ -2181,7 +2181,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>75</v>
       </c>
@@ -2198,7 +2198,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>61</v>
       </c>
@@ -2215,7 +2215,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>48</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>76</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>62</v>
       </c>
@@ -2266,7 +2266,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>9</v>
       </c>
@@ -2280,7 +2280,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>32</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6</v>
       </c>
@@ -2308,7 +2308,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>51</v>
       </c>
@@ -2325,7 +2325,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>79</v>
       </c>
@@ -2342,7 +2342,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>65</v>
       </c>
@@ -2359,7 +2359,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>20</v>
       </c>
@@ -2376,7 +2376,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>21</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -2410,7 +2410,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>98</v>
       </c>
@@ -2424,7 +2424,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>22</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>95</v>
       </c>
@@ -2455,7 +2455,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>97</v>
       </c>
@@ -2469,7 +2469,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>52</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>80</v>
       </c>
@@ -2503,7 +2503,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>66</v>
       </c>
@@ -2520,7 +2520,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>93</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>53</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>81</v>
       </c>
@@ -2571,7 +2571,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>67</v>
       </c>
@@ -2588,7 +2588,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>44</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>45</v>
       </c>
@@ -2622,7 +2622,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>46</v>
       </c>
@@ -2639,7 +2639,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>28</v>
       </c>
@@ -2653,7 +2653,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>107</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>108</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>109</v>
       </c>
@@ -2695,7 +2695,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>110</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>111</v>
       </c>
@@ -2723,7 +2723,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>112</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>113</v>
       </c>
@@ -2751,7 +2751,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>114</v>
       </c>
@@ -2765,7 +2765,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>115</v>
       </c>
@@ -2779,7 +2779,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>116</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>99</v>
       </c>
@@ -2807,7 +2807,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>117</v>
       </c>
@@ -2821,7 +2821,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>118</v>
       </c>
@@ -2835,7 +2835,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>100</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>101</v>
       </c>
@@ -2863,7 +2863,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>102</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>103</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>104</v>
       </c>
@@ -2905,7 +2905,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>105</v>
       </c>
@@ -2919,7 +2919,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>106</v>
       </c>
@@ -2933,7 +2933,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>30</v>
       </c>
@@ -2947,7 +2947,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>26</v>
       </c>
@@ -2961,7 +2961,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>25</v>
       </c>
@@ -2975,7 +2975,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>7</v>
       </c>
@@ -2989,7 +2989,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>8</v>
       </c>
@@ -3003,7 +3003,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>29</v>
       </c>
@@ -3017,7 +3017,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>27</v>
       </c>
@@ -3031,7 +3031,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>54</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>82</v>
       </c>
@@ -3065,7 +3065,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>68</v>
       </c>
@@ -3082,7 +3082,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>55</v>
       </c>
@@ -3099,7 +3099,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>83</v>
       </c>
@@ -3116,7 +3116,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>69</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>89</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>36</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>90</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>56</v>
       </c>
@@ -3201,7 +3201,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>84</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>70</v>
       </c>
@@ -3235,7 +3235,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>42</v>
       </c>
@@ -3249,7 +3249,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>39</v>
       </c>
@@ -3263,7 +3263,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>57</v>
       </c>
@@ -3280,7 +3280,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>85</v>
       </c>
@@ -3297,7 +3297,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>71</v>
       </c>
@@ -3314,7 +3314,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>58</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>86</v>
       </c>
@@ -3348,7 +3348,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>72</v>
       </c>
@@ -3365,7 +3365,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>5</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>16</v>
       </c>
@@ -3393,7 +3393,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>17</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>18</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>15</v>
       </c>
@@ -3435,7 +3435,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>14</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>59</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>87</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>73</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>60</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>88</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>74</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>94</v>
       </c>
@@ -3565,7 +3565,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>96</v>
       </c>
@@ -3579,7 +3579,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>31</v>
       </c>
@@ -3593,7 +3593,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>43</v>
       </c>
@@ -3607,7 +3607,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>24</v>
       </c>
@@ -3621,7 +3621,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>40</v>
       </c>
@@ -3635,7 +3635,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>41</v>
       </c>
@@ -3649,7 +3649,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>37</v>
       </c>
@@ -3663,7 +3663,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>38</v>
       </c>
@@ -3677,7 +3677,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>19</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>33</v>
       </c>
@@ -3708,7 +3708,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>34</v>
       </c>
@@ -3722,7 +3722,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>1</v>
       </c>
@@ -3736,7 +3736,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>2</v>
       </c>
@@ -3750,7 +3750,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>91</v>
       </c>
@@ -3767,7 +3767,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>92</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>35</v>
       </c>
@@ -3798,7 +3798,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>49</v>
       </c>
@@ -3815,7 +3815,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>77</v>
       </c>
@@ -3832,7 +3832,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>63</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>50</v>
       </c>
@@ -3866,7 +3866,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>78</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>64</v>
       </c>
@@ -3900,7 +3900,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>125</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>126</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>127</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>128</v>
       </c>
@@ -3969,9 +3969,6 @@
       <c r="A128">
         <v>129</v>
       </c>
-      <c r="B128" t="s">
-        <v>204</v>
-      </c>
       <c r="C128" t="s">
         <v>214</v>
       </c>
@@ -3982,7 +3979,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>130</v>
       </c>
@@ -3996,7 +3993,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>131</v>
       </c>
@@ -4013,7 +4010,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>132</v>
       </c>
@@ -4030,7 +4027,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>133</v>
       </c>
@@ -4044,7 +4041,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>134</v>
       </c>
@@ -4058,7 +4055,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>135</v>
       </c>
@@ -4072,7 +4069,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>136</v>
       </c>
@@ -4086,7 +4083,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>137</v>
       </c>
@@ -4100,7 +4097,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>138</v>
       </c>
@@ -4114,7 +4111,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>139</v>
       </c>
@@ -4128,7 +4125,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>140</v>
       </c>
@@ -4145,7 +4142,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>141</v>
       </c>
@@ -5349,10 +5346,10 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E220">
+  <autoFilter ref="A1:E220" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
-        <filter val="application_{train|test}.csv"/>
+        <filter val="bureau.csv"/>
       </filters>
     </filterColumn>
     <sortState ref="A2:E123">

</xml_diff>

<commit_message>
more progress with processing bureau and bureau_balance
</commit_message>
<xml_diff>
--- a/input/HomeCredit_columns_description.xlsx
+++ b/input/HomeCredit_columns_description.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackr\Documents\kaggle\kaggle-home-credit-default-risk\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{772C0E52-7264-42E7-93E2-67F9E0642073}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FA2B165D-5840-4905-A25C-F969ADE6A658}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1860" yWindow="0" windowWidth="27870" windowHeight="12810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1998,7 +1998,7 @@
   <dimension ref="A1:E220"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D131" sqref="D131"/>
+      <selection activeCell="D143" sqref="D143"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3900,7 +3900,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>125</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>126</v>
       </c>
@@ -3934,7 +3934,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>127</v>
       </c>
@@ -3948,7 +3948,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>128</v>
       </c>
@@ -3979,7 +3979,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>130</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>131</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>132</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>133</v>
       </c>
@@ -4041,7 +4041,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>134</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>135</v>
       </c>
@@ -4069,7 +4069,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>136</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>137</v>
       </c>
@@ -4097,7 +4097,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>138</v>
       </c>
@@ -4111,7 +4111,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>139</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>140</v>
       </c>
@@ -4142,7 +4142,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>141</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="141" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>142</v>
       </c>
@@ -4173,7 +4173,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="142" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>143</v>
       </c>
@@ -4190,7 +4190,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="143" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>144</v>
       </c>
@@ -5349,7 +5349,7 @@
   <autoFilter ref="A1:E220" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
-        <filter val="bureau.csv"/>
+        <filter val="bureau_balance.csv"/>
       </filters>
     </filterColumn>
     <sortState ref="A2:E123">

</xml_diff>